<commit_message>
added new recipes, fixed burrito bowls
</commit_message>
<xml_diff>
--- a/source/recipes.xlsx
+++ b/source/recipes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Github\GF_Repo\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EE650E-7CF5-4827-830A-6C24129463CB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336210B6-190D-4901-8BB2-39375F7C4DC9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="135" windowWidth="17235" windowHeight="7230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,13 +152,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,28 +592,78 @@
       <c r="B6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
+      <c r="A7"/>
+      <c r="B7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>